<commit_message>
Se crea función que resta horas
</commit_message>
<xml_diff>
--- a/resultado_consulta.xlsx
+++ b/resultado_consulta.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P179"/>
+  <dimension ref="A1:Q179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +518,11 @@
           <t>producto</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>tipo_producto</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -574,6 +579,11 @@
           <t>Vertical Mixta 2 puertas</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -630,6 +640,11 @@
           <t>Mesa auxiliar caliente</t>
         </is>
       </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -686,6 +701,11 @@
           <t>Mesa auxilia bar</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -742,6 +762,11 @@
           <t>Parrilla Industrial</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -798,6 +823,11 @@
           <t>Mueble Lava Traperos</t>
         </is>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -854,6 +884,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -910,6 +945,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -966,6 +1006,11 @@
           <t>Plancha Sobre poner</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1022,6 +1067,11 @@
           <t>Estufa de Sobre poner</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1078,6 +1128,11 @@
           <t>Mesa auxiliar caliente</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1130,6 +1185,11 @@
         </is>
       </c>
       <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1186,6 +1246,11 @@
           <t>Freidora 2 Canastillas Individuales</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1242,6 +1307,11 @@
           <t>Mesa lavado + Shuts</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1298,6 +1368,11 @@
           <t>Base Chef Refrigerada</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1354,6 +1429,11 @@
           <t>Mesa con lavado</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1406,6 +1486,11 @@
         </is>
       </c>
       <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1458,6 +1543,11 @@
         </is>
       </c>
       <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1514,6 +1604,11 @@
           <t>Congelador vertical 1 Puerta</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1570,6 +1665,11 @@
           <t>Congelador vertical 1 Puerta</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1626,6 +1726,11 @@
           <t>Plancha Industrial</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1682,6 +1787,11 @@
           <t>Estufa Industrial 6 Puestos</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1738,6 +1848,11 @@
           <t>Freidora 2 Canastillas</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1790,6 +1905,11 @@
           <t>Nevera 2 Puertas</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1846,6 +1966,11 @@
           <t>Nevera 2 Puertas</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1902,6 +2027,11 @@
           <t>Freidora 2 Canastillas</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1954,6 +2084,11 @@
         </is>
       </c>
       <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2006,6 +2141,11 @@
         </is>
       </c>
       <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2058,6 +2198,11 @@
         </is>
       </c>
       <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2116,6 +2261,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2172,6 +2322,11 @@
           <t>Mesa auxiliar lavado</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2230,6 +2385,11 @@
           <t>Vitrina Tipo Loft</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2286,6 +2446,11 @@
           <t>Campana Industrial cuadrada</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2332,6 +2497,11 @@
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2388,6 +2558,11 @@
           <t>Repisa Entrada/Salida platos</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2446,6 +2621,11 @@
           <t>Mesa con lavado</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2504,6 +2684,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2562,6 +2747,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2620,6 +2810,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2676,6 +2871,11 @@
           <t>Mueble Lava Traperos</t>
         </is>
       </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2728,6 +2928,11 @@
           <t>Lamina acero puertas</t>
         </is>
       </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2784,6 +2989,11 @@
           <t>Mesa lavado + Shuts</t>
         </is>
       </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2840,6 +3050,11 @@
           <t>Vitrina Tipo Loft</t>
         </is>
       </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2896,6 +3111,11 @@
           <t>carcamo de bar</t>
         </is>
       </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2952,6 +3172,11 @@
           <t>Vitrina Tipo Loft</t>
         </is>
       </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3008,6 +3233,11 @@
           <t>Repisa Entrada/Salida platos</t>
         </is>
       </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3064,6 +3294,11 @@
           <t>Carcamos de piso</t>
         </is>
       </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3120,6 +3355,11 @@
           <t>Carcamos de piso</t>
         </is>
       </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3176,6 +3416,11 @@
           <t>Carcamos de piso</t>
         </is>
       </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3234,6 +3479,11 @@
           <t>Adicionales Bar</t>
         </is>
       </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3286,6 +3536,11 @@
           <t>Mesa con lavado menaje</t>
         </is>
       </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3342,6 +3597,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3394,6 +3654,11 @@
           <t>Mueble con lavado bar</t>
         </is>
       </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3446,6 +3711,11 @@
           <t>Mueble shuts</t>
         </is>
       </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3498,6 +3768,11 @@
           <t>Campana Industrial cuadrada</t>
         </is>
       </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3550,6 +3825,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3602,6 +3882,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3658,6 +3943,11 @@
           <t>Refrigerador vertical 1 puerta</t>
         </is>
       </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3710,6 +4000,11 @@
         </is>
       </c>
       <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3766,6 +4061,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3822,6 +4122,11 @@
           <t>mueble de lavado con puertas</t>
         </is>
       </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3878,6 +4183,11 @@
           <t>Punto de pago</t>
         </is>
       </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3934,6 +4244,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3990,6 +4305,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4046,6 +4366,11 @@
           <t>Logistica, transporte, accesorios e instalacion</t>
         </is>
       </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4102,6 +4427,11 @@
           <t>Estacion de bar en congelacion</t>
         </is>
       </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4158,6 +4488,11 @@
           <t>Freidora 2 Tanques, 3 canastillas</t>
         </is>
       </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4214,6 +4549,11 @@
           <t>Congelador vertical 1 Puerta</t>
         </is>
       </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -4270,6 +4610,11 @@
           <t>Mesa auxiliar lavado</t>
         </is>
       </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -4326,6 +4671,11 @@
           <t>Campana Industrial cuadrada</t>
         </is>
       </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -4382,6 +4732,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4438,6 +4793,11 @@
           <t>Mesa auxiliar caliente</t>
         </is>
       </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4490,6 +4850,11 @@
           <t>Mesa en Isla</t>
         </is>
       </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4546,6 +4911,11 @@
           <t>Campana Industrial cuadrada</t>
         </is>
       </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4602,6 +4972,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4658,6 +5033,11 @@
           <t>Freidora 2 Tanques, 4 canastillas</t>
         </is>
       </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4714,6 +5094,11 @@
           <t>Congelador Horizontal</t>
         </is>
       </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4770,6 +5155,11 @@
           <t>Mesa de auxiliar  curva Plantillada</t>
         </is>
       </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4826,6 +5216,11 @@
           <t>Motor tipo Hongo</t>
         </is>
       </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4882,6 +5277,11 @@
           <t>Logistica, transporte, accesorios e instalacion</t>
         </is>
       </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4938,6 +5338,11 @@
           <t>Estacion de bar seca</t>
         </is>
       </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4994,6 +5399,11 @@
           <t>Estacion de bar congelacion</t>
         </is>
       </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -5050,6 +5460,11 @@
           <t>Arrancador Motor 2Hp</t>
         </is>
       </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -5106,6 +5521,11 @@
           <t>Parrilla Industrial a carbon</t>
         </is>
       </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -5162,6 +5582,11 @@
           <t>Sistema de ducteria</t>
         </is>
       </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -5218,6 +5643,11 @@
           <t>Plancha Sobre poner</t>
         </is>
       </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -5274,6 +5704,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -5330,6 +5765,11 @@
           <t>Estufa de Sobre poner</t>
         </is>
       </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -5386,6 +5826,11 @@
           <t>Campana Industrial cuadrada</t>
         </is>
       </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -5442,6 +5887,11 @@
           <t>pozuelo de lavado</t>
         </is>
       </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5494,6 +5944,11 @@
           <t>Base Chef Refrigerada</t>
         </is>
       </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5550,6 +6005,11 @@
           <t>Estacion de bar seca</t>
         </is>
       </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -5602,6 +6062,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -5654,6 +6119,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5706,6 +6176,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -5758,6 +6233,11 @@
           <t>Repisa Entrada/Salida platos</t>
         </is>
       </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5810,6 +6290,11 @@
           <t>Repisa Entrada/Salida platos</t>
         </is>
       </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5862,6 +6347,11 @@
           <t>Mesa auxiliar lavado</t>
         </is>
       </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5914,6 +6404,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5966,6 +6461,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -6018,6 +6518,11 @@
           <t>Congelador Horizontal</t>
         </is>
       </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -6074,6 +6579,11 @@
           <t>Estufa Enana</t>
         </is>
       </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -6130,6 +6640,11 @@
           <t>Mesa con lavado</t>
         </is>
       </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -6186,6 +6701,11 @@
           <t>Refrigerador vertical 1 puerta</t>
         </is>
       </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -6242,6 +6762,11 @@
           <t>Mesa de apoyo</t>
         </is>
       </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -6298,6 +6823,11 @@
           <t>Mueble shuts</t>
         </is>
       </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -6354,6 +6884,11 @@
           <t>Mueble con lavado bar</t>
         </is>
       </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -6410,6 +6945,11 @@
           <t>Estacion de Licuado</t>
         </is>
       </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -6466,6 +7006,11 @@
           <t>Mesa de apoyo</t>
         </is>
       </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -6522,6 +7067,11 @@
           <t>Mesa auxiliar caliente</t>
         </is>
       </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -6574,6 +7124,11 @@
           <t>Campana Industrial cuadrada</t>
         </is>
       </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -6626,6 +7181,11 @@
           <t>Refrigerador vertical 1 puerta</t>
         </is>
       </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -6678,6 +7238,11 @@
           <t>Mesa con lavado menaje</t>
         </is>
       </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -6730,6 +7295,11 @@
           <t>Escurridor de Loza</t>
         </is>
       </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -6786,6 +7356,11 @@
           <t>Vitrina Tipo Loft</t>
         </is>
       </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -6842,6 +7417,11 @@
           <t>Campana Industrial cuadrada</t>
         </is>
       </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -6898,6 +7478,11 @@
           <t>Punto de pago</t>
         </is>
       </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -6954,6 +7539,11 @@
           <t>Vitrina Tipo Loft</t>
         </is>
       </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -7010,6 +7600,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -7066,6 +7661,11 @@
           <t>Plancha Industrial</t>
         </is>
       </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -7122,6 +7722,11 @@
           <t>Estufa Industrial 6 Puestos</t>
         </is>
       </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -7178,6 +7783,11 @@
           <t>repisa industrial</t>
         </is>
       </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -7234,6 +7844,11 @@
           <t>Escurridor de Loza</t>
         </is>
       </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -7290,6 +7905,11 @@
           <t>Mesa en Isla</t>
         </is>
       </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -7346,6 +7966,11 @@
           <t>freidora 1 Canastilla</t>
         </is>
       </c>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -7402,6 +8027,11 @@
           <t>Estacion de bar</t>
         </is>
       </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -7458,6 +8088,11 @@
           <t>Mesa con lavado</t>
         </is>
       </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -7516,6 +8151,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -7572,6 +8212,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -7628,6 +8273,11 @@
           <t>Estacion de bar congelacion</t>
         </is>
       </c>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -7684,6 +8334,11 @@
           <t>Mueble con puertas</t>
         </is>
       </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -7740,6 +8395,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -7796,6 +8456,11 @@
           <t>Mesa con lavado</t>
         </is>
       </c>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -7852,6 +8517,11 @@
           <t>Estacion de bar congelacion</t>
         </is>
       </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -7910,6 +8580,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -7966,6 +8641,11 @@
           <t>Congelador vertical 1 Puerta</t>
         </is>
       </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -8024,6 +8704,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -8082,6 +8767,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -8140,6 +8830,11 @@
           <t>Estanteria industrial</t>
         </is>
       </c>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -8196,6 +8891,11 @@
           <t>Refrigerador Horizontal</t>
         </is>
       </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -8252,6 +8952,11 @@
           <t>Mesa auxilia bar</t>
         </is>
       </c>
+      <c r="Q141" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -8308,6 +9013,11 @@
           <t>Mesa auxilia bar</t>
         </is>
       </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -8360,6 +9070,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -8412,6 +9127,11 @@
           <t>Base para mantenedor</t>
         </is>
       </c>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -8470,6 +9190,11 @@
           <t>Modulo Mixto a gas</t>
         </is>
       </c>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -8522,6 +9247,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -8574,6 +9304,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -8626,6 +9361,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -8678,6 +9418,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -8730,6 +9475,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -8782,6 +9532,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -8834,6 +9589,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q152" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -8886,6 +9646,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -8938,6 +9703,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -8990,6 +9760,11 @@
           <t>repisa industrial</t>
         </is>
       </c>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -9042,6 +9817,11 @@
           <t>Mesa de apoyo</t>
         </is>
       </c>
+      <c r="Q156" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -9094,6 +9874,11 @@
           <t>Mesa de apoyo</t>
         </is>
       </c>
+      <c r="Q157" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -9146,6 +9931,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -9198,6 +9988,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -9250,6 +10045,11 @@
           <t>Mesa de apoyo</t>
         </is>
       </c>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -9302,6 +10102,11 @@
           <t>Mesa con lavado</t>
         </is>
       </c>
+      <c r="Q161" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -9354,6 +10159,11 @@
           <t>Mesa con lavado</t>
         </is>
       </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -9406,6 +10216,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -9458,6 +10273,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -9510,6 +10330,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -9562,6 +10387,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -9618,6 +10448,11 @@
           <t>Congelador Horizontal</t>
         </is>
       </c>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -9670,6 +10505,11 @@
           <t>Mesa de trabajo</t>
         </is>
       </c>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -9722,6 +10562,11 @@
           <t>Reformas</t>
         </is>
       </c>
+      <c r="Q169" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -9778,6 +10623,11 @@
           <t>Baño maria de servicio</t>
         </is>
       </c>
+      <c r="Q170" t="inlineStr">
+        <is>
+          <t>coccion</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -9834,6 +10684,11 @@
           <t>Campana Industrial cuadrada</t>
         </is>
       </c>
+      <c r="Q171" t="inlineStr">
+        <is>
+          <t>extraccion</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -9890,6 +10745,11 @@
           <t>Tapa removible</t>
         </is>
       </c>
+      <c r="Q172" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -9942,6 +10802,11 @@
           <t>bandeja recolectora agua</t>
         </is>
       </c>
+      <c r="Q173" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -9998,6 +10863,11 @@
           <t>Reformas</t>
         </is>
       </c>
+      <c r="Q174" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -10052,6 +10922,11 @@
           <t>Estacion de bar seca</t>
         </is>
       </c>
+      <c r="Q175" t="inlineStr">
+        <is>
+          <t>carpinteria</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -10106,6 +10981,11 @@
           <t>Congelador Horizontal</t>
         </is>
       </c>
+      <c r="Q176" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -10160,6 +11040,11 @@
           <t>Congelador Horizontal</t>
         </is>
       </c>
+      <c r="Q177" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -10216,6 +11101,11 @@
           <t>Cava de Vinos</t>
         </is>
       </c>
+      <c r="Q178" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -10272,6 +11162,11 @@
           <t>Cava de Vinos</t>
         </is>
       </c>
+      <c r="Q179" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>